<commit_message>
pushing new eda2 & processing2files
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D73D0D88-3017-429D-A793-87FC1DE0BC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D25D409-A645-794C-8BB3-88D0A0FA5B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="2438" windowWidth="14400" windowHeight="8182" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="1640" windowWidth="14400" windowHeight="8180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>Height</t>
   </si>
@@ -80,22 +80,28 @@
     <t>Hair Color</t>
   </si>
   <si>
-    <t>Blonde</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>Brown</t>
-  </si>
-  <si>
-    <t>White</t>
-  </si>
-  <si>
-    <t>Purple</t>
+    <t>How many strands of hair the individual has</t>
+  </si>
+  <si>
+    <t>What color the invididual's hair is</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>BR/BL/R/W/P; BR=brown, BL= black, R= red, W= white, P= purple</t>
   </si>
 </sst>
 </file>
@@ -424,13 +430,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,7 +453,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>180</v>
       </c>
@@ -461,10 +467,10 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>175</v>
       </c>
@@ -478,10 +484,10 @@
         <v>5000</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -498,7 +504,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>178</v>
       </c>
@@ -515,7 +521,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>192</v>
       </c>
@@ -532,7 +538,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -546,10 +552,10 @@
         <v>8000</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>156</v>
       </c>
@@ -563,10 +569,10 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>166</v>
       </c>
@@ -583,7 +589,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>155</v>
       </c>
@@ -600,7 +606,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>145</v>
       </c>
@@ -617,7 +623,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>165</v>
       </c>
@@ -628,10 +634,10 @@
         <v>6050</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>133</v>
       </c>
@@ -648,7 +654,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>166</v>
       </c>
@@ -665,7 +671,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>154</v>
       </c>
@@ -689,20 +695,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.265625" customWidth="1"/>
-    <col min="3" max="3" width="21.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -713,7 +719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -724,7 +730,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -735,7 +741,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -744,6 +750,28 @@
       </c>
       <c r="C4" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merge conflict fix attempt
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9ADCF9-A80D-4D42-B7B7-3CC3B0E421CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D25D409-A645-794C-8BB3-88D0A0FA5B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1177" yWindow="1635" windowWidth="14400" windowHeight="8183" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="1640" windowWidth="14400" windowHeight="8180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -434,9 +434,9 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,7 +453,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>180</v>
       </c>
@@ -470,7 +470,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>175</v>
       </c>
@@ -487,7 +487,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -504,7 +504,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>178</v>
       </c>
@@ -521,7 +521,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>192</v>
       </c>
@@ -538,7 +538,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -555,7 +555,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>156</v>
       </c>
@@ -572,7 +572,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>166</v>
       </c>
@@ -589,7 +589,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>155</v>
       </c>
@@ -606,7 +606,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>145</v>
       </c>
@@ -623,7 +623,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>165</v>
       </c>
@@ -637,7 +637,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>133</v>
       </c>
@@ -654,7 +654,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>166</v>
       </c>
@@ -671,7 +671,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>154</v>
       </c>
@@ -701,14 +701,14 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.265625" customWidth="1"/>
-    <col min="3" max="3" width="21.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -719,7 +719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -730,7 +730,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -741,7 +741,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -752,7 +752,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -763,7 +763,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>

</xml_diff>